<commit_message>
updated patch panel mapping for A/44
</commit_message>
<xml_diff>
--- a/PatchPanel.xlsx
+++ b/PatchPanel.xlsx
@@ -250,10 +250,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
@@ -372,10 +372,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix rack moxa cabling records
</commit_message>
<xml_diff>
--- a/PatchPanel.xlsx
+++ b/PatchPanel.xlsx
@@ -246,14 +246,14 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
@@ -773,7 +773,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,10 +787,10 @@
         <v>35</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>